<commit_message>
added trade info into regression, improved regression, tried to remove outliers did not improve regression
</commit_message>
<xml_diff>
--- a/Resources/Data/Production_Data/country_market_months.xlsx
+++ b/Resources/Data/Production_Data/country_market_months.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grothjd/DS_bootcamp/Project_1_Coffee_Price_Predictors/Resources/Data/Production_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98C4D32D-4030-E44F-B729-EA164C77C31C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B5F904-AE0B-4B49-80CA-E7409EC888FC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16340" xr2:uid="{B404FC9D-021B-7148-8616-7F586DFC06AC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Angola</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Country_Name</t>
+  </si>
+  <si>
+    <t>Month_Start</t>
+  </si>
+  <si>
+    <t>Month_End</t>
   </si>
 </sst>
 </file>
@@ -520,7 +526,7 @@
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,6 +538,12 @@
       <c r="A1" t="s">
         <v>46</v>
       </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">

</xml_diff>